<commit_message>
Adding User and Email features
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_register.xlsx
+++ b/reports/templates/reportTemplate_register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="972" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3520206-101B-41E9-A7E2-2CC48463B786}"/>
+  <xr:revisionPtr revIDLastSave="1004" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{185AB6A7-73CD-45F0-96B8-6A382CD199B7}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="18930" windowWidth="21600" windowHeight="11385" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
+    <workbookView xWindow="4215" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="218">
   <si>
     <t>Preadvise ID</t>
   </si>
@@ -696,6 +696,24 @@
   <si>
     <t>Share of tenders involved in the following tradelanes</t>
   </si>
+  <si>
+    <t>Average time between reception &amp; registration</t>
+  </si>
+  <si>
+    <t>Average time between registration &amp; Deadline Rd.1</t>
+  </si>
+  <si>
+    <t>Outcome Positive</t>
+  </si>
+  <si>
+    <t>Outcome negative</t>
+  </si>
+  <si>
+    <t>Outcome unknown</t>
+  </si>
+  <si>
+    <t>Is over ?</t>
+  </si>
 </sst>
 </file>
 
@@ -705,10 +723,10 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00&quot; TEU(s)&quot;_-;\-* #,##0.00&quot; TEU(s)&quot;_-;_-* &quot;-&quot;??&quot; TEU(s)&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot; Ton(s)&quot;_-;\-* #,##0.00&quot; Ton(s)&quot;_-;_-* &quot;-&quot;??&quot; Ton(s)&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00&quot; CMB(s)&quot;_-;\-* #,##0.00&quot; CBM(s)&quot;_-;_-* &quot;-&quot;??&quot; CBM(s)&quot;_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00&quot; month(s)&quot;_-;\-* #,##0.00&quot; month(s)&quot;_-;_-* &quot;-&quot;??&quot; month(s)&quot;_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0&quot; day(s)&quot;_-;\-* #,##0&quot; day(s)&quot;_-;_-* &quot;-&quot;??&quot; day(s)&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00&quot; month(s)&quot;_-;\-* #,##0.00&quot; month(s)&quot;_-;_-* &quot;-&quot;??&quot; month(s)&quot;_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0&quot; day(s)&quot;_-;\-* #,##0&quot; day(s)&quot;_-;_-* &quot;-&quot;??&quot; day(s)&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1011,10 +1029,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1040,9 +1058,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EF5C85F-01A4-46CF-9039-EFF5C6FFD4F7}" name="DataTable" displayName="DataTable" ref="A1:CT3" totalsRowShown="0">
-  <autoFilter ref="A1:CT3" xr:uid="{9EF5C85F-01A4-46CF-9039-EFF5C6FFD4F7}"/>
-  <tableColumns count="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EF5C85F-01A4-46CF-9039-EFF5C6FFD4F7}" name="DataTable" displayName="DataTable" ref="A1:CZ3" totalsRowShown="0">
+  <autoFilter ref="A1:CZ3" xr:uid="{9EF5C85F-01A4-46CF-9039-EFF5C6FFD4F7}"/>
+  <tableColumns count="104">
     <tableColumn id="1" xr3:uid="{2CB6E984-6BB5-4D7A-A81F-D0601EB90E6A}" name="Register ID"/>
     <tableColumn id="2" xr3:uid="{6FFAC53E-7EFD-47C3-8EFB-8BCEA51789AA}" name="Record date"/>
     <tableColumn id="3" xr3:uid="{A2764E2D-9117-429E-9F02-FB27FCC1E6DA}" name="Last modified date"/>
@@ -1141,6 +1159,16 @@
     <tableColumn id="43" xr3:uid="{F0A3C84D-B3DA-4A33-B398-CC7FA56D5327}" name="Amount of awardee(s)"/>
     <tableColumn id="95" xr3:uid="{B92014CC-6E49-4451-9E2C-F869F7E1D72A}" name="Decision criteria"/>
     <tableColumn id="96" xr3:uid="{44E237BF-A768-4D13-8426-F53B0C0E94F1}" name="Feedback available"/>
+    <tableColumn id="91" xr3:uid="{F400EDA5-7EA1-4E72-9A69-5D9320F44822}" name="Average time between reception &amp; registration">
+      <calculatedColumnFormula>DATEDIF(DataTable[[#This Row],[Tender reception date]],DataTable[[#This Row],[Record date]],"d")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="100" xr3:uid="{BBDB0AE8-F51A-4459-A0EB-25C7C4A1A773}" name="Average time between registration &amp; Deadline Rd.1">
+      <calculatedColumnFormula>DATEDIF(DataTable[[#This Row],[Record date]],DataTable[[#This Row],[Tender deadline]],"d")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="101" xr3:uid="{867BAAB6-4A29-4B40-B477-9FE8034A8470}" name="Is over ?"/>
+    <tableColumn id="102" xr3:uid="{36ACCB0A-0703-43F6-ABCE-F5FC4CDAE992}" name="Outcome Positive"/>
+    <tableColumn id="103" xr3:uid="{556D5C2B-E560-4D59-AA98-C52AAAFB9392}" name="Outcome negative"/>
+    <tableColumn id="104" xr3:uid="{5A5025E9-A518-44B9-A5DF-106E1ABCBA1A}" name="Outcome unknown"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1351,11 +1379,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F65E63-F005-4CBF-AE0A-8C9CDC031092}">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A64" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="60.125" customWidth="1"/>
     <col min="2" max="2" width="24.25" customWidth="1"/>
@@ -1364,7 +1392,7 @@
     <col min="8" max="13" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -1386,10 +1414,10 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1406,19 +1434,19 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="B5" s="1"/>
       <c r="H5" s="28" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>124</v>
       </c>
@@ -1429,7 +1457,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1">
       <c r="B7" s="1"/>
       <c r="I7" s="8" t="s">
         <v>61</v>
@@ -1447,7 +1475,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1481,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15" customHeight="1">
       <c r="B9" s="1"/>
       <c r="H9" s="11" t="s">
         <v>57</v>
@@ -1507,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1539,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15" customHeight="1">
       <c r="B11" s="1"/>
       <c r="H11" s="11" t="s">
         <v>59</v>
@@ -1565,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1604,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1620,7 +1648,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15" customHeight="1">
       <c r="A14" t="s">
         <v>162</v>
       </c>
@@ -1630,7 +1658,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15" customHeight="1">
       <c r="B15" s="1"/>
       <c r="H15" s="10" t="s">
         <v>71</v>
@@ -1644,7 +1672,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15" customHeight="1">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -1660,7 +1688,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1679,7 +1707,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1695,7 +1723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="B19" s="1"/>
       <c r="I19" s="8" t="s">
         <v>61</v>
@@ -1713,7 +1741,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1732,27 +1760,27 @@
         <v>56</v>
       </c>
       <c r="I20" s="13">
-        <f>I8/$B$10</f>
+        <f t="shared" ref="I20:M24" si="1">I8/$B$10</f>
         <v>0</v>
       </c>
       <c r="J20" s="14">
-        <f>J8/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K20" s="14">
-        <f>K8/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L20" s="14">
-        <f>L8/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M20" s="15">
-        <f>M8/$B$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1771,27 +1799,27 @@
         <v>57</v>
       </c>
       <c r="I21" s="13">
-        <f>I9/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J21" s="14">
-        <f>J9/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K21" s="14">
-        <f>K9/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L21" s="14">
-        <f>L9/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M21" s="15">
-        <f>M9/$B$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -1810,27 +1838,27 @@
         <v>58</v>
       </c>
       <c r="I22" s="13">
-        <f>I10/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J22" s="14">
-        <f>J10/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K22" s="14">
-        <f>K10/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L22" s="14">
-        <f>L10/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M22" s="15">
-        <f>M10/$B$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1849,27 +1877,27 @@
         <v>59</v>
       </c>
       <c r="I23" s="13">
-        <f>I11/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J23" s="14">
-        <f>J11/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K23" s="14">
-        <f>K11/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L23" s="14">
-        <f>L11/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M23" s="15">
-        <f>M11/$B$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" customHeight="1">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1888,27 +1916,27 @@
         <v>60</v>
       </c>
       <c r="I24" s="16">
-        <f>I12/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J24" s="17">
-        <f>J12/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K24" s="17">
-        <f>K12/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L24" s="17">
-        <f>L12/$B$10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M24" s="18">
-        <f>M12/$B$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -1924,7 +1952,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1940,7 +1968,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" customHeight="1">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1956,7 +1984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15" customHeight="1">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1972,7 +2000,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -1988,7 +2016,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" customHeight="1">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2004,7 +2032,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="15" customHeight="1">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2020,7 +2048,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -2036,7 +2064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2052,10 +2080,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1">
       <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
@@ -2066,10 +2094,10 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2085,7 +2113,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2101,7 +2129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15" customHeight="1">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2117,7 +2145,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15" customHeight="1">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2133,10 +2161,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15" customHeight="1">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15" customHeight="1">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2145,7 +2173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15" customHeight="1">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2154,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="15" customHeight="1">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -2163,7 +2191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="15" customHeight="1">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -2172,10 +2200,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="15" customHeight="1">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="15" customHeight="1">
       <c r="A47" t="s">
         <v>131</v>
       </c>
@@ -2184,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="15" customHeight="1">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2193,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="15" customHeight="1">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -2202,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="15" customHeight="1">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -2211,8 +2239,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15" customHeight="1"/>
+    <row r="52" spans="1:7" ht="15.75" thickBot="1">
       <c r="A52" s="7" t="s">
         <v>66</v>
       </c>
@@ -2223,7 +2251,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="15">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -2239,7 +2267,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="15">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -2255,7 +2283,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="15">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -2271,7 +2299,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="15">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -2287,7 +2315,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="15">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -2303,7 +2331,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15">
       <c r="A60" s="10" t="s">
         <v>72</v>
       </c>
@@ -2314,7 +2342,7 @@
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="15">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -2330,7 +2358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="15">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -2346,7 +2374,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="15">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -2362,19 +2390,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="15">
       <c r="B64" s="1"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="15">
       <c r="B65" s="1"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="15">
       <c r="B66" s="1"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="15">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -2390,7 +2418,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="15">
       <c r="A68" t="s">
         <v>102</v>
       </c>
@@ -2406,7 +2434,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="15">
       <c r="A69" t="s">
         <v>103</v>
       </c>
@@ -2422,7 +2450,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="15">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -2438,7 +2466,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="15">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -2454,7 +2482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="15">
       <c r="A73" t="s">
         <v>106</v>
       </c>
@@ -2470,7 +2498,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="15">
       <c r="A74" t="s">
         <v>107</v>
       </c>
@@ -2486,7 +2514,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="15">
       <c r="A75" t="s">
         <v>109</v>
       </c>
@@ -2502,7 +2530,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="15">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -2518,7 +2546,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1">
       <c r="A78" s="7" t="s">
         <v>110</v>
       </c>
@@ -2529,7 +2557,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="15">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -2545,7 +2573,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="15">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -2561,7 +2589,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="15">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -2577,7 +2605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="15">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -2593,7 +2621,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1">
       <c r="A85" s="7" t="s">
         <v>116</v>
       </c>
@@ -2604,7 +2632,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="15">
       <c r="A87" t="s">
         <v>111</v>
       </c>
@@ -2620,7 +2648,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="15">
       <c r="A88" t="s">
         <v>114</v>
       </c>
@@ -2636,7 +2664,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="15">
       <c r="A89" t="s">
         <v>113</v>
       </c>
@@ -2652,7 +2680,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="15">
       <c r="A90" t="s">
         <v>112</v>
       </c>
@@ -2668,7 +2696,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="15">
       <c r="A91" t="s">
         <v>115</v>
       </c>
@@ -2684,7 +2712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="15">
       <c r="A93" t="s">
         <v>117</v>
       </c>
@@ -2700,7 +2728,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="15">
       <c r="A94" t="s">
         <v>118</v>
       </c>
@@ -2716,7 +2744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="15">
       <c r="A95" t="s">
         <v>119</v>
       </c>
@@ -2732,7 +2760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="15">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -2748,7 +2776,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="15">
       <c r="A97" t="s">
         <v>121</v>
       </c>
@@ -2764,7 +2792,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="15" customHeight="1">
       <c r="A99" t="s">
         <v>122</v>
       </c>
@@ -2780,7 +2808,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="15">
       <c r="A100" t="s">
         <v>123</v>
       </c>
@@ -2796,7 +2824,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="17.25" thickBot="1">
       <c r="A101" s="2" t="s">
         <v>125</v>
       </c>
@@ -2807,8 +2835,8 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="15" thickTop="1"/>
+    <row r="103" spans="1:7" ht="15.75" thickBot="1">
       <c r="A103" s="7" t="s">
         <v>126</v>
       </c>
@@ -2819,19 +2847,25 @@
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="15">
       <c r="A105" t="s">
         <v>127</v>
       </c>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B105" s="30">
+        <f>IFERROR(AVERAGE(Data!CU:CU),"-")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15">
       <c r="A106" t="s">
         <v>160</v>
       </c>
-      <c r="B106" s="1"/>
-    </row>
-    <row r="108" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="30" t="str">
+        <f>IFERROR(AVERAGE(Data!CV:CV),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" thickBot="1">
       <c r="A108" s="7" t="s">
         <v>136</v>
       </c>
@@ -2842,7 +2876,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="15">
       <c r="A110" t="s">
         <v>128</v>
       </c>
@@ -2851,7 +2885,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="15">
       <c r="A111" t="s">
         <v>129</v>
       </c>
@@ -2860,7 +2894,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="15.75" thickBot="1">
       <c r="A113" s="7" t="s">
         <v>137</v>
       </c>
@@ -2871,7 +2905,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="15">
       <c r="A115" t="s">
         <v>138</v>
       </c>
@@ -2880,14 +2914,14 @@
         <v>0</v>
       </c>
       <c r="D115" s="6">
-        <f t="shared" ref="D115:D122" si="1">$B115/$B$10</f>
+        <f t="shared" ref="D115:D122" si="2">$B115/$B$10</f>
         <v>0</v>
       </c>
       <c r="E115" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="15">
       <c r="A116" t="s">
         <v>139</v>
       </c>
@@ -2896,14 +2930,14 @@
         <v>0</v>
       </c>
       <c r="D116" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E116" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="15">
       <c r="A117" t="s">
         <v>140</v>
       </c>
@@ -2912,14 +2946,14 @@
         <v>0</v>
       </c>
       <c r="D117" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E117" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="15">
       <c r="A118" t="s">
         <v>141</v>
       </c>
@@ -2928,14 +2962,14 @@
         <v>0</v>
       </c>
       <c r="D118" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E118" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="15">
       <c r="A119" t="s">
         <v>142</v>
       </c>
@@ -2944,14 +2978,14 @@
         <v>0</v>
       </c>
       <c r="D119" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E119" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="15">
       <c r="A120" t="s">
         <v>143</v>
       </c>
@@ -2960,14 +2994,14 @@
         <v>0</v>
       </c>
       <c r="D120" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E120" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="15">
       <c r="A121" t="s">
         <v>144</v>
       </c>
@@ -2976,14 +3010,14 @@
         <v>0</v>
       </c>
       <c r="D121" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E121" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="15">
       <c r="A122" t="s">
         <v>145</v>
       </c>
@@ -2992,14 +3026,14 @@
         <v>0</v>
       </c>
       <c r="D122" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E122" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="15.75" thickBot="1">
       <c r="A124" s="7" t="s">
         <v>146</v>
       </c>
@@ -3010,7 +3044,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="15">
       <c r="A126" t="s">
         <v>147</v>
       </c>
@@ -3026,7 +3060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="15">
       <c r="A127" t="s">
         <v>148</v>
       </c>
@@ -3042,7 +3076,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="15">
       <c r="A128" t="s">
         <v>149</v>
       </c>
@@ -3058,7 +3092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" ht="15">
       <c r="A129" t="s">
         <v>150</v>
       </c>
@@ -3074,7 +3108,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15">
       <c r="A130" t="s">
         <v>151</v>
       </c>
@@ -3104,20 +3138,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408FA63C-ED69-49C0-8A89-D58054A38125}">
-  <dimension ref="A1:CT3"/>
+  <dimension ref="A1:CZ3"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1048537" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="CU2" sqref="CU2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="98" width="22.875" customWidth="1"/>
-    <col min="99" max="99" width="28" customWidth="1"/>
-    <col min="100" max="100" width="19" customWidth="1"/>
+    <col min="99" max="104" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:104">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -3412,8 +3445,26 @@
       <c r="CT1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="CU1" t="s">
+        <v>212</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>213</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>217</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>214</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>215</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:104">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3552,8 +3603,16 @@
       <c r="CM2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="CU2">
+        <f>DATEDIF(DataTable[[#This Row],[Tender reception date]],DataTable[[#This Row],[Record date]],"d")</f>
+        <v>1</v>
+      </c>
+      <c r="CV2" t="e">
+        <f>DATEDIF(DataTable[[#This Row],[Record date]],DataTable[[#This Row],[Tender deadline]],"d")</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:104">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3691,6 +3750,14 @@
       </c>
       <c r="CM3">
         <v>1</v>
+      </c>
+      <c r="CU3">
+        <f>DATEDIF(DataTable[[#This Row],[Tender reception date]],DataTable[[#This Row],[Record date]],"d")</f>
+        <v>1</v>
+      </c>
+      <c r="CV3" t="e">
+        <f>DATEDIF(DataTable[[#This Row],[Record date]],DataTable[[#This Row],[Tender deadline]],"d")</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification of the Register Excel template
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_register.xlsx
+++ b/reports/templates/reportTemplate_register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1028" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB314B04-128E-417D-ACDD-360B22B04290}"/>
+  <xr:revisionPtr revIDLastSave="1030" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89BC76CB-955B-47D7-8790-75ED6AF9C20F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
+    <workbookView xWindow="-25035" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -729,7 +729,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.00&quot; month(s)&quot;_-;\-* #,##0.00&quot; month(s)&quot;_-;_-* &quot;-&quot;??&quot; month(s)&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0&quot; day(s)&quot;_-;\-* #,##0&quot; day(s)&quot;_-;_-* &quot;-&quot;??&quot; day(s)&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1385,9 +1385,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F65E63-F005-4CBF-AE0A-8C9CDC031092}">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.125" customWidth="1"/>
     <col min="2" max="2" width="22.875" customWidth="1"/>
@@ -1398,7 +1400,7 @@
     <col min="16" max="16" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -1420,10 +1422,10 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1">
+    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1442,7 +1444,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1450,13 +1452,13 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="H5" s="28" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>124</v>
       </c>
@@ -1467,7 +1469,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="I7" s="8" t="s">
         <v>61</v>
@@ -1485,7 +1487,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="H9" s="11" t="s">
         <v>57</v>
@@ -1545,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1577,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="H11" s="11" t="s">
         <v>59</v>
@@ -1603,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1658,7 +1660,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>162</v>
       </c>
@@ -1668,7 +1670,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="H15" s="10" t="s">
         <v>71</v>
@@ -1682,7 +1684,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -1698,7 +1700,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1717,7 +1719,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="I19" s="8" t="s">
         <v>61</v>
@@ -1751,7 +1753,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1790,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -1868,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1">
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1946,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1">
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -1962,7 +1964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1">
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1994,7 +1996,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1">
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2010,7 +2012,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1">
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -2026,7 +2028,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1">
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2058,7 +2060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1">
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -2074,7 +2076,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2090,10 +2092,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
@@ -2104,10 +2106,10 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2123,7 +2125,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2155,7 +2157,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2171,10 +2173,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2183,7 +2185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -2201,7 +2203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -2210,10 +2212,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>131</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1">
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1">
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -2240,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1">
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -2249,8 +2251,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1"/>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1">
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>66</v>
       </c>
@@ -2261,7 +2263,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="54" spans="1:7" ht="15">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -2277,7 +2279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -2293,7 +2295,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -2309,7 +2311,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -2325,7 +2327,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>72</v>
       </c>
@@ -2352,7 +2354,7 @@
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="1:7" ht="15">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -2368,7 +2370,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -2400,19 +2402,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:7" ht="15">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="1:7" ht="15">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:7" ht="15">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>102</v>
       </c>
@@ -2444,7 +2446,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>103</v>
       </c>
@@ -2460,7 +2462,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -2476,7 +2478,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -2492,7 +2494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>106</v>
       </c>
@@ -2508,7 +2510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>107</v>
       </c>
@@ -2524,7 +2526,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>109</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -2556,7 +2558,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>110</v>
       </c>
@@ -2567,7 +2569,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="80" spans="1:7" ht="15">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -2583,7 +2585,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -2599,7 +2601,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -2631,7 +2633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>116</v>
       </c>
@@ -2642,7 +2644,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="87" spans="1:7" ht="15">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>111</v>
       </c>
@@ -2658,7 +2660,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>114</v>
       </c>
@@ -2674,7 +2676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>113</v>
       </c>
@@ -2690,7 +2692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>112</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>115</v>
       </c>
@@ -2722,7 +2724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>117</v>
       </c>
@@ -2738,7 +2740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>118</v>
       </c>
@@ -2754,7 +2756,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>119</v>
       </c>
@@ -2770,7 +2772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -2786,7 +2788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>121</v>
       </c>
@@ -2802,7 +2804,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1">
+    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>122</v>
       </c>
@@ -2818,7 +2820,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>123</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="17.25" thickBot="1">
+    <row r="101" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>125</v>
       </c>
@@ -2845,8 +2847,8 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" ht="15" thickTop="1"/>
-    <row r="103" spans="1:7" ht="15.75" thickBot="1">
+    <row r="102" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>126</v>
       </c>
@@ -2857,25 +2859,25 @@
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="105" spans="1:7" ht="15">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>127</v>
       </c>
       <c r="B105" s="30">
-        <f>IFERROR(AVERAGE(Data!CU:CU),"-")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15">
+        <f>IFERROR(ABS(AVERAGE(Data!CU:CU)),"-")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>160</v>
       </c>
       <c r="B106" s="30" t="str">
-        <f>IFERROR(AVERAGE(Data!CV:CV),"-")</f>
+        <f>IFERROR(ABS(AVERAGE(Data!CV:CV)),"-")</f>
         <v>-</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15.75" thickBot="1">
+    <row r="108" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>136</v>
       </c>
@@ -2886,7 +2888,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="15">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>128</v>
       </c>
@@ -2895,7 +2897,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>129</v>
       </c>
@@ -2904,7 +2906,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15.75" thickBot="1">
+    <row r="113" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>137</v>
       </c>
@@ -2915,7 +2917,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
     </row>
-    <row r="115" spans="1:7" ht="15">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>138</v>
       </c>
@@ -2931,7 +2933,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>139</v>
       </c>
@@ -2947,7 +2949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>140</v>
       </c>
@@ -2963,7 +2965,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>141</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>142</v>
       </c>
@@ -2995,7 +2997,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>143</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>144</v>
       </c>
@@ -3027,7 +3029,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>145</v>
       </c>
@@ -3043,7 +3045,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15.75" thickBot="1">
+    <row r="124" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>146</v>
       </c>
@@ -3054,7 +3056,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
     </row>
-    <row r="126" spans="1:7" ht="15">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>147</v>
       </c>
@@ -3070,7 +3072,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>148</v>
       </c>
@@ -3086,7 +3088,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>149</v>
       </c>
@@ -3102,7 +3104,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>150</v>
       </c>
@@ -3118,7 +3120,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>151</v>
       </c>
@@ -3154,13 +3156,13 @@
       <selection activeCell="CU2" sqref="CU2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="98" width="22.875" customWidth="1"/>
     <col min="99" max="104" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104">
+    <row r="1" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -3474,7 +3476,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:104">
+    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3622,7 +3624,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:104">
+    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Minor changes on register excel templates formulas
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_register.xlsx
+++ b/reports/templates/reportTemplate_register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1030" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89BC76CB-955B-47D7-8790-75ED6AF9C20F}"/>
+  <xr:revisionPtr revIDLastSave="1035" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DFC8081-9F71-4CE6-9792-8C1885CC7013}"/>
   <bookViews>
-    <workbookView xWindow="-25035" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -2729,7 +2729,7 @@
         <v>117</v>
       </c>
       <c r="B93" s="1">
-        <f>COUNTIF(Data!CR2:CR1048576,"Price competitiveness")</f>
+        <f>COUNTIF(Data!CS2:CS1048576,"Price competitiveness")</f>
         <v>0</v>
       </c>
       <c r="D93" s="6">
@@ -2745,7 +2745,7 @@
         <v>118</v>
       </c>
       <c r="B94" s="1">
-        <f>COUNTIF(Data!CR2:CR1048576,"History with the company")</f>
+        <f>COUNTIF(Data!CS2:CS1048576,"History with the company")</f>
         <v>0</v>
       </c>
       <c r="D94" s="6">
@@ -2761,7 +2761,7 @@
         <v>119</v>
       </c>
       <c r="B95" s="1">
-        <f>COUNTIF(Data!CR2:CR1048576,"Ability to answer to all lanes")</f>
+        <f>COUNTIF(Data!CS2:CS1048576,"Ability to answer to all lanes")</f>
         <v>0</v>
       </c>
       <c r="D95" s="6">
@@ -2777,7 +2777,7 @@
         <v>120</v>
       </c>
       <c r="B96" s="1">
-        <f>COUNTIF(Data!CR2:CR1048576,"Ability to provide an extended offer")</f>
+        <f>COUNTIF(Data!CS2:CS1048576,"Ability to provide an extended offer")</f>
         <v>0</v>
       </c>
       <c r="D96" s="6">
@@ -2793,7 +2793,7 @@
         <v>121</v>
       </c>
       <c r="B97" s="1">
-        <f>COUNTIFS(Data!CR2:CR1048576,"Unknown",Data!CR2:CR1048576,"")</f>
+        <f>COUNTIFS(Data!CS2:CS1048576,"Unknown",Data!CR2:CR1048576,"")</f>
         <v>0</v>
       </c>
       <c r="D97" s="6">
@@ -3152,7 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408FA63C-ED69-49C0-8A89-D58054A38125}">
   <dimension ref="A1:CZ3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="CM1" workbookViewId="0">
       <selection activeCell="CU2" sqref="CU2"/>
     </sheetView>
   </sheetViews>

</xml_diff>